<commit_message>
changed company data sheet to update financial field name.
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waqar Ahmad\Desktop\git\codencode-site\Code-N-Code.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E666648-C7A1-4E56-BD81-F8179450911A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7785F899-CC6F-4BBA-9D9A-547B89E1FAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -145,9 +145,6 @@
     <t>https://www.linkedin.com/company/swiggy-in/?originalSubdomain=in</t>
   </si>
   <si>
-    <t xml:space="preserve">Financial </t>
-  </si>
-  <si>
     <t>https://www.bseindia.com/xml-data/corpfiling/AttachHis/48dd15e3-9bdf-4d67-90e0-83c08e4cd048.pdf</t>
   </si>
   <si>
@@ -259,6 +256,9 @@
   </si>
   <si>
     <t>18 Jan 2010</t>
+  </si>
+  <si>
+    <t>Financial</t>
   </si>
 </sst>
 </file>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -804,25 +804,25 @@
         <v>33</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>38</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -946,21 +946,21 @@
         <v>40</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="29.4" thickBot="1">
       <c r="A4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="D4" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>15</v>
@@ -974,14 +974,14 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -990,28 +990,28 @@
       </c>
       <c r="Q4" s="6"/>
       <c r="R4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="S4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="S4" s="11" t="s">
+      <c r="T4" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="T4" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="U4" s="6"/>
     </row>
     <row r="5" spans="1:21" ht="72.599999999999994" thickBot="1">
       <c r="A5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="D5" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>16</v>
@@ -1029,14 +1029,14 @@
         <v>21</v>
       </c>
       <c r="J5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
@@ -1046,27 +1046,27 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
       <c r="S5" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="T5" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="U5" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="U5" s="12" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="58.2" thickBot="1">
       <c r="A6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="D6" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>16</v>
@@ -1084,30 +1084,30 @@
         <v>21</v>
       </c>
       <c r="J6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="S6" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="S6" s="12" t="s">
-        <v>74</v>
       </c>
       <c r="T6" s="6"/>
       <c r="U6" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated code to show proper company logo.
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waqar Ahmad\Desktop\git\codencode-site\Code-N-Code.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waqar Ahmad\Desktop\git\ajay\CompanyMasterData.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A453DEA8-689A-485C-8ED7-172872891121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52016B6C-054B-4F55-B662-8BB2D857BEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
   <si>
     <t>Company Name</t>
   </si>
@@ -259,6 +259,24 @@
   </si>
   <si>
     <t>Financial</t>
+  </si>
+  <si>
+    <t>Image Url</t>
+  </si>
+  <si>
+    <t>Byjus.png</t>
+  </si>
+  <si>
+    <t>Swiggy Access.png</t>
+  </si>
+  <si>
+    <t>Lenskart.png</t>
+  </si>
+  <si>
+    <t>Mamaearth.png</t>
+  </si>
+  <si>
+    <t>zomato.png</t>
   </si>
 </sst>
 </file>
@@ -733,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+      <selection activeCell="V1" sqref="V1:V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -761,9 +779,10 @@
     <col min="19" max="19" width="21.109375" customWidth="1"/>
     <col min="20" max="20" width="33.44140625" customWidth="1"/>
     <col min="21" max="21" width="35.33203125" customWidth="1"/>
+    <col min="22" max="22" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -824,8 +843,11 @@
       <c r="U1" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="V1" s="6" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22" ht="15" thickBot="1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -886,8 +908,11 @@
       <c r="U2" t="s">
         <v>19</v>
       </c>
+      <c r="V2" s="6" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" ht="15" thickBot="1">
+    <row r="3" spans="1:22" ht="43.8" thickBot="1">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -948,8 +973,11 @@
       <c r="U3" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="V3" s="6" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" ht="29.4" thickBot="1">
+    <row r="4" spans="1:22" ht="29.4" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>47</v>
       </c>
@@ -999,8 +1027,11 @@
         <v>55</v>
       </c>
       <c r="U4" s="6"/>
+      <c r="V4" s="6" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" ht="72.599999999999994" thickBot="1">
+    <row r="5" spans="1:22" ht="72.599999999999994" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>56</v>
       </c>
@@ -1054,8 +1085,11 @@
       <c r="U5" s="12" t="s">
         <v>64</v>
       </c>
+      <c r="V5" s="6" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" ht="58.2" thickBot="1">
+    <row r="6" spans="1:22" ht="58.2" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>65</v>
       </c>
@@ -1108,6 +1142,9 @@
       <c r="T6" s="6"/>
       <c r="U6" s="12" t="s">
         <v>74</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new company data.
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waqar Ahmad\Desktop\git\ajay\CompanyMasterData.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52016B6C-054B-4F55-B662-8BB2D857BEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D223208-D799-471C-8E0A-541C12A15FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="132">
   <si>
     <t>Company Name</t>
   </si>
@@ -277,13 +277,154 @@
   </si>
   <si>
     <t>zomato.png</t>
+  </si>
+  <si>
+    <t>Delhivery Ltd.</t>
+  </si>
+  <si>
+    <t>Delhivery</t>
+  </si>
+  <si>
+    <t>L63090DL2011PLC221234</t>
+  </si>
+  <si>
+    <t>Integrated Freight &amp; Logistics</t>
+  </si>
+  <si>
+    <t>Delhivery Limited, founded in 2011 and based in Gurugram, India, is a publicly listed integrated logistics and supply-chain technology provider. It offers express parcel and heavy-goods delivery, part-truckload and truckload freight, warehousing, cross-border logistics, and value-added services such as return handling, payment collection, fraud detection, and supply-chain software, serving e-commerce, retail, FMCG, automotive, and manufacturing sectors across India</t>
+  </si>
+  <si>
+    <t>N24-N34, S24-S34, Air Cargo Logistics Centre-II, Opposite Gate 6 Cargo Terminal, IGI Airport, New Delhi, Delhi, India - 110037.</t>
+  </si>
+  <si>
+    <t>91-124-6225602</t>
+  </si>
+  <si>
+    <t>corporate@delhivery.com</t>
+  </si>
+  <si>
+    <t>https://www.delhivery.com/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/company/delhivery?originalSubdomain=in</t>
+  </si>
+  <si>
+    <t>https://www.bseindia.com/xml-data/corpfiling/AttachHis/83f3f0e7-c1a2-405a-96be-da9c383369d8.pdf</t>
+  </si>
+  <si>
+    <t>ANI Technologies Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>Ola Cabs, OlaCabs</t>
+  </si>
+  <si>
+    <t>U72900KA2010PTC086596</t>
+  </si>
+  <si>
+    <t>Trucking, Passenger Ground Transportation</t>
+  </si>
+  <si>
+    <t>Ola Consumer (formerly Ola Cabs), founded in December 2010 and headquartered in Bangalore, is India’s largest mobility platform, serving over 250 cities. It provides ride-hailing across vehicles like bikes, autos, and cabs, and has expanded into verticals such as financial services, micro-insurance, cloud kitchens, and fleet management. The company emphasizes technological innovation and digital integration to streamline urban transportation</t>
+  </si>
+  <si>
+    <t>Ola Campus, Wing C, Prestige RMZ Startech, Hosur Road, Municipal Ward No. 67, Industrial Layout, Koramangala VI Bk, Bangalore South, Karnataka, India, 560095</t>
+  </si>
+  <si>
+    <t>2, Hosur Rd, Koramangala Industrial Layout, Koramangala, Bengaluru, Karnataka 560095</t>
+  </si>
+  <si>
+    <t>91-80-41437121</t>
+  </si>
+  <si>
+    <t>https://www.olacabs.com/</t>
+  </si>
+  <si>
+    <t>Delightful Gourmet Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>licious</t>
+  </si>
+  <si>
+    <t>U74900KA2015PTC080321</t>
+  </si>
+  <si>
+    <t>Packaged Foods &amp; Meats</t>
+  </si>
+  <si>
+    <t>Licious, founded in 2015 and headquartered in Bengaluru, is an India-based D2C brand offering fresh meat, seafood, ready-to-cook, and ready-to-eat products through a farm-to-fork model. It controls its supply and cold chain, ensuring hygiene and freshness across multiple Indian cities.</t>
+  </si>
+  <si>
+    <t>Maruti Infotech Center No. 11/1, 12/1, Tower A, Ground Floor, Amarjyothi Layout, Intermediate Ring Road, Domlur, Bangalore North, Karnataka, India, 560071</t>
+  </si>
+  <si>
+    <t>talktous@licious.com</t>
+  </si>
+  <si>
+    <t>https://www.licious.in/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/company/licious/about/</t>
+  </si>
+  <si>
+    <t>OFB Tech Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>ofbusiness</t>
+  </si>
+  <si>
+    <t>U74140GJ2015PTC154393</t>
+  </si>
+  <si>
+    <t>Trading Companies &amp; Distributors</t>
+  </si>
+  <si>
+    <t>OfBusiness, founded in 2015, is an Indian B2B fintech platform headquartered in Gurugram. It aggregates raw materials—such as metals, chemicals, agriculture products, and apparel—and provides SME-focused financing and contract manufacturing services. The company integrates procurement, private-label manufacturing, and working capital solutions to streamline supply chains and enhance pricing efficiency for businesses.</t>
+  </si>
+  <si>
+    <t>B-1102, Sankalp Iconic Tower, Opp. Vikram Nagar, Bopal Ambli Road, Bodakdev, Ahmedabad, Ahmadabad City, Gujarat, India, 380054</t>
+  </si>
+  <si>
+    <t>91-011-41054262</t>
+  </si>
+  <si>
+    <t>82975 85873</t>
+  </si>
+  <si>
+    <t>contact@ofbusiness.com</t>
+  </si>
+  <si>
+    <t>https://www.ofbusiness.com/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/company/10485930/</t>
+  </si>
+  <si>
+    <t>delhivery.png</t>
+  </si>
+  <si>
+    <t>ola.png</t>
+  </si>
+  <si>
+    <t>licious.png</t>
+  </si>
+  <si>
+    <t>ofbusiness.png</t>
+  </si>
+  <si>
+    <t>22 Jun 2011</t>
+  </si>
+  <si>
+    <t>13 May 2015</t>
+  </si>
+  <si>
+    <t>24 Aug 2015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +479,12 @@
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="MyFirstFont"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF080809"/>
+      <name val="Segoe UI Historic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -397,7 +544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -445,6 +592,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -751,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:V6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -912,7 +1068,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="43.8" thickBot="1">
+    <row r="3" spans="1:22" ht="15" thickBot="1">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1146,6 +1302,250 @@
       <c r="V6" s="6" t="s">
         <v>84</v>
       </c>
+    </row>
+    <row r="7" spans="1:22" ht="29.4" thickBot="1">
+      <c r="A7" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="13">
+        <v>543529</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="L7" s="6"/>
+      <c r="M7" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="101.4" thickBot="1">
+      <c r="A8" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="29.4" thickBot="1">
+      <c r="A9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L9" s="6"/>
+      <c r="M9" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="S9" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="30.6" thickBot="1">
+      <c r="A10" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="M10" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="P10" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="T10" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15" thickBot="1">
+      <c r="A11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1161,8 +1561,17 @@
     <hyperlink ref="U5" r:id="rId10" xr:uid="{CF2FB9B2-4AD0-4339-B08D-D48E55484907}"/>
     <hyperlink ref="S6" r:id="rId11" xr:uid="{8712A85A-E5C7-4922-95B3-95CE20CF7C84}"/>
     <hyperlink ref="U6" r:id="rId12" xr:uid="{FF2FF4A2-FFD8-46D9-907D-65CAC3E55A0A}"/>
+    <hyperlink ref="S7" r:id="rId13" xr:uid="{86278C4C-A691-4658-8A66-4D4B0B934D56}"/>
+    <hyperlink ref="T7" r:id="rId14" xr:uid="{93CCAF74-BA45-4A4F-B657-C456D4E5E542}"/>
+    <hyperlink ref="U7" r:id="rId15" xr:uid="{A650C2C7-5B85-4535-93C6-CB5C65BC561C}"/>
+    <hyperlink ref="S8" r:id="rId16" xr:uid="{8ACD0C66-82CD-4925-A77B-8B98D241E239}"/>
+    <hyperlink ref="R9" r:id="rId17" display="mailto:talktous@licious.com" xr:uid="{714C65FD-FBA9-4604-BD32-5B91CAEB5C59}"/>
+    <hyperlink ref="S9" r:id="rId18" xr:uid="{B2247057-11D2-4EB6-8F76-8BF7172FDDF9}"/>
+    <hyperlink ref="T9" r:id="rId19" xr:uid="{88CE51AF-43F4-4223-B391-6B1D1B28D374}"/>
+    <hyperlink ref="S10" r:id="rId20" xr:uid="{08E7C937-2948-4258-8B1E-C918E84EEB08}"/>
+    <hyperlink ref="T10" r:id="rId21" xr:uid="{E56695D8-D013-4C2B-A62F-98DDAC80ECDA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added unacademy company data.
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waqar Ahmad\Desktop\git\ajay\CompanyMasterData.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D223208-D799-471C-8E0A-541C12A15FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C53F109-3B3E-41FE-AC06-E75E0195EB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="139">
   <si>
     <t>Company Name</t>
   </si>
@@ -418,6 +418,27 @@
   </si>
   <si>
     <t>24 Aug 2015</t>
+  </si>
+  <si>
+    <t>Sorting Hat Technologies Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>Unacademy</t>
+  </si>
+  <si>
+    <t>U72200KA2015PTC082063</t>
+  </si>
+  <si>
+    <t>Education Services</t>
+  </si>
+  <si>
+    <t>https://unacademy.com/</t>
+  </si>
+  <si>
+    <t>unacademy.png</t>
+  </si>
+  <si>
+    <t>6 Aug 2015</t>
   </si>
 </sst>
 </file>
@@ -544,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -592,9 +613,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -910,7 +928,7 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1313,7 +1331,7 @@
       <c r="C7" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>129</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -1373,7 +1391,7 @@
       <c r="C8" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>77</v>
       </c>
       <c r="E8" s="6" t="s">
@@ -1425,7 +1443,7 @@
       <c r="C9" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>130</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -1477,7 +1495,7 @@
       <c r="C10" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>131</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -1505,7 +1523,7 @@
       <c r="O10" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="P10" s="19" t="s">
+      <c r="P10" s="18" t="s">
         <v>121</v>
       </c>
       <c r="Q10" s="6"/>
@@ -1523,29 +1541,51 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="15" thickBot="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+    <row r="11" spans="1:22" ht="29.4" thickBot="1">
+      <c r="A11" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="J11" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
+      <c r="P11" s="6">
+        <v>8585858585</v>
+      </c>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
-      <c r="S11" s="12"/>
+      <c r="S11" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
+      <c r="V11" s="6" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1570,8 +1610,9 @@
     <hyperlink ref="T9" r:id="rId19" xr:uid="{88CE51AF-43F4-4223-B391-6B1D1B28D374}"/>
     <hyperlink ref="S10" r:id="rId20" xr:uid="{08E7C937-2948-4258-8B1E-C918E84EEB08}"/>
     <hyperlink ref="T10" r:id="rId21" xr:uid="{E56695D8-D013-4C2B-A62F-98DDAC80ECDA}"/>
+    <hyperlink ref="S11" r:id="rId22" xr:uid="{86140607-8330-459C-8398-0BE42D33304F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added logs for debugging.
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waqar Ahmad\Desktop\git\ajay\CompanyMasterData.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7916A3-9E62-443E-8E55-81EA8B55F17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861360CD-CFD3-46CA-AC6E-ADA5CE2FC538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -928,7 +928,7 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>